<commit_message>
menu and choice conditions are finished. todo: calculation mechanism
</commit_message>
<xml_diff>
--- a/core/data_base/type_gran.xlsx
+++ b/core/data_base/type_gran.xlsx
@@ -14,19 +14,13 @@
   <sheets>
     <sheet name="type_gran" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>code_mehs</t>
-  </si>
-  <si>
-    <t>name_mehs</t>
-  </si>
-  <si>
     <t>Песок рыхлый</t>
   </si>
   <si>
@@ -52,16 +46,28 @@
   </si>
   <si>
     <t>Глина тяжелая</t>
+  </si>
+  <si>
+    <t>code_meh</t>
+  </si>
+  <si>
+    <t>name_meh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -85,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -437,16 +444,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -462,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -470,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -478,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -486,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -494,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -502,7 +515,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -510,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -518,7 +531,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>